<commit_message>
thêm đơn hàng trực tiếp vào báo cáo kpi
</commit_message>
<xml_diff>
--- a/DMS/Templates/KpiGeneral_Employee_Report.xlsx
+++ b/DMS/Templates/KpiGeneral_Employee_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45106A7-7AB1-407F-89F6-068B9F7320EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AFBD96-6E13-4096-B7A4-13B5290FE80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>STT</t>
   </si>
@@ -154,6 +154,54 @@
   </si>
   <si>
     <t>{{KpiGeneralEmployeeReports.KpiYear}}</t>
+  </si>
+  <si>
+    <t>Số đơn hàng trực tiếp</t>
+  </si>
+  <si>
+    <t>Tổng sản lượng theo đơn trực tiếp</t>
+  </si>
+  <si>
+    <t>Doanh thu theo đơn trực tiếp</t>
+  </si>
+  <si>
+    <t>SKU/Đơn hàng trực tiếp</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectOrdersPLanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectOrders}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectOrdersRatio}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectQuantityPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectQuantity}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectQuantityRatio}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectSalesAmountPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectSalesAmount}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalDirectSalesAmountRatio}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.SkuDirectOrderPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.SkuDirectOrder}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.SkuDirectOrderRatio}}</t>
   </si>
 </sst>
 </file>
@@ -297,6 +345,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,12 +366,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,89 +647,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="12.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.44140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="14.33203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.44140625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="12.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
+    <col min="21" max="22" width="14.28515625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" style="1" customWidth="1"/>
+    <col min="26" max="27" width="14.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.42578125" style="1" customWidth="1"/>
+    <col min="31" max="32" width="13.85546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
+    <col min="34" max="35" width="14.85546875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
-    <row r="4" spans="1:24" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:36" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -703,56 +760,76 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="6" t="s">
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6" t="s">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6" t="s">
+      <c r="T7" s="9"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T7" s="7"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="W7" s="7"/>
-      <c r="X7" s="8"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="10"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
@@ -816,96 +893,172 @@
       <c r="X8" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="Y8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="N9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="O9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="P9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="Q9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="R9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="S9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="T9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="U9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="V9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="W9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="X9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="S9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="V9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="W9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="X9" s="12" t="s">
-        <v>40</v>
+      <c r="Y9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+  <mergeCells count="17">
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A4:U4"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="V7:X7"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:U4"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="AH7:AJ7"/>
+    <mergeCell ref="V7:X7"/>
     <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="Y7:AA7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix báo cáo kpi
</commit_message>
<xml_diff>
--- a/DMS/Templates/KpiGeneral_Employee_Report.xlsx
+++ b/DMS/Templates/KpiGeneral_Employee_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RangDong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AFBD96-6E13-4096-B7A4-13B5290FE80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50BE91D-0008-4825-849A-2E4F01212465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -653,43 +653,43 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="12.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="14.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" style="1" customWidth="1"/>
-    <col min="26" max="27" width="14.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="13.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="14.42578125" style="1" customWidth="1"/>
-    <col min="31" max="32" width="13.85546875" style="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
-    <col min="34" max="35" width="14.85546875" style="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="14.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
+    <col min="13" max="14" width="12.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.25" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.75" style="1" customWidth="1"/>
+    <col min="21" max="22" width="14.25" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="14.125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.375" style="1" customWidth="1"/>
+    <col min="31" max="32" width="13.875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.75" style="1" customWidth="1"/>
+    <col min="34" max="35" width="14.875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14.125" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -771,37 +771,37 @@
         <v>13</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="10"/>
       <c r="J7" s="8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="10"/>
       <c r="M7" s="8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="10"/>
       <c r="P7" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="10"/>
       <c r="S7" s="8" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="T7" s="9"/>
       <c r="U7" s="10"/>
       <c r="V7" s="8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="W7" s="9"/>
       <c r="X7" s="10"/>
@@ -941,67 +941,67 @@
         <v>42</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="R9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="S9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="U9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="V9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="W9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="X9" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="V9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="Y9" s="7" t="s">
         <v>47</v>
@@ -1042,23 +1042,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A4:U4"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="S7:U7"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
     <mergeCell ref="AB7:AD7"/>
     <mergeCell ref="AE7:AG7"/>
     <mergeCell ref="AH7:AJ7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Y7:AA7"/>
     <mergeCell ref="V7:X7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="Y7:AA7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
thêm các trạng thái mới KPI general
</commit_message>
<xml_diff>
--- a/DMS/Templates/KpiGeneral_Employee_Report.xlsx
+++ b/DMS/Templates/KpiGeneral_Employee_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD86EE8-D7A8-4EE2-9E37-503C06609454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C260E65-961E-47D8-A648-B11048B4861C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -42,18 +42,9 @@
     <t>Kỳ KPI</t>
   </si>
   <si>
-    <t>Số đơn hàng gián tiếp</t>
-  </si>
-  <si>
-    <t>Tổng sản lượng theo đơn gián tiếp</t>
-  </si>
-  <si>
     <t>Doanh thu theo đơn gián tiếp</t>
   </si>
   <si>
-    <t>SKU/Đơn hàng gián tiếp</t>
-  </si>
-  <si>
     <t>Kế hoạch</t>
   </si>
   <si>
@@ -69,15 +60,6 @@
     <t>Năm KPI</t>
   </si>
   <si>
-    <t>Số đại lý viếng thăm</t>
-  </si>
-  <si>
-    <t>Số đại lý tạo mới</t>
-  </si>
-  <si>
-    <t>Số lần viếng thăm đại lý</t>
-  </si>
-  <si>
     <t>{{Username}}</t>
   </si>
   <si>
@@ -87,24 +69,6 @@
     <t>{{KpiGeneralEmployeeReports.STT}}</t>
   </si>
   <si>
-    <t>{{KpiGeneralEmployeeReports.TotalIndirectOrdersPLanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalIndirectOrders}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalIndirectOrdersRatio}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalIndirectQuantityPlanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalIndirectQuantity}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalIndirectQuantityRatio}}</t>
-  </si>
-  <si>
     <t>{{KpiGeneralEmployeeReports.TotalIndirectSalesAmountPlanned}}</t>
   </si>
   <si>
@@ -114,15 +78,6 @@
     <t>{{KpiGeneralEmployeeReports.TotalIndirectSalesAmountRatio}}</t>
   </si>
   <si>
-    <t>{{KpiGeneralEmployeeReports.SkuIndirectOrderPlanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.SkuIndirectOrder}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.SkuIndirectOrderRatio}}</t>
-  </si>
-  <si>
     <t>{{KpiGeneralEmployeeReports.StoresVisitedPLanned}}</t>
   </si>
   <si>
@@ -150,58 +105,91 @@
     <t>{{KpiGeneralEmployeeReports.NumberOfStoreVisitsRatio}}</t>
   </si>
   <si>
-    <t>Số đơn hàng trực tiếp</t>
-  </si>
-  <si>
-    <t>Tổng sản lượng theo đơn trực tiếp</t>
-  </si>
-  <si>
-    <t>Doanh thu theo đơn trực tiếp</t>
-  </si>
-  <si>
-    <t>SKU/Đơn hàng trực tiếp</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectOrdersPLanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectOrders}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectOrdersRatio}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectQuantityPlanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectQuantity}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectQuantityRatio}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectSalesAmountPlanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectSalesAmount}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.TotalDirectSalesAmountRatio}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.SkuDirectOrderPlanned}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.SkuDirectOrder}}</t>
-  </si>
-  <si>
-    <t>{{KpiGeneralEmployeeReports.SkuDirectOrderRatio}}</t>
-  </si>
-  <si>
     <t>{{KpiGeneralEmployeeReports.KpiYearName}}</t>
   </si>
   <si>
     <t>{{KpiGeneralEmployeeReports.KpiPeriodName}}</t>
+  </si>
+  <si>
+    <t>Doanh thu C2 Trọng điểm</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2TDPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2TD}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2TDRatio}}</t>
+  </si>
+  <si>
+    <t>Doanh thu C2 Siêu lớn</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2SLPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2SL}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2SLRatio}}</t>
+  </si>
+  <si>
+    <t>Doanh thu C2</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2Planned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.RevenueC2Ratio}}</t>
+  </si>
+  <si>
+    <t>Tổng số đại lý mở mới</t>
+  </si>
+  <si>
+    <t>Số đại lý trọng điểm mở mới</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.NewStoreC2CreatedPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.NewStoreC2Created}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.NewStoreC2CreatedRatio}}</t>
+  </si>
+  <si>
+    <t>Số đại lý ghé thăm</t>
+  </si>
+  <si>
+    <t>Tổng số lượt ghé thăm</t>
+  </si>
+  <si>
+    <t>Số thông tin phản ánh</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalProblemPlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalProblemCreated}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalProblemRatio}}</t>
+  </si>
+  <si>
+    <t>Số hình ảnh chụp</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalImagePlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalImageCreated}}</t>
+  </si>
+  <si>
+    <t>{{KpiGeneralEmployeeReports.TotalImageRatio}}</t>
   </si>
 </sst>
 </file>
@@ -216,7 +204,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -654,52 +642,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="12.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="14.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" style="1" customWidth="1"/>
-    <col min="26" max="27" width="14.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="13.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="14.42578125" style="1" customWidth="1"/>
-    <col min="31" max="32" width="13.85546875" style="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
-    <col min="34" max="35" width="14.85546875" style="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="14.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
+    <col min="13" max="14" width="12.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.25" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.75" style="1" customWidth="1"/>
+    <col min="21" max="22" width="14.25" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="14.125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.375" style="1" customWidth="1"/>
+    <col min="31" max="32" width="13.875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.75" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -709,7 +695,7 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -717,9 +703,9 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="4" spans="1:36" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -745,7 +731,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -755,19 +741,19 @@
         <v>1</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -775,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>5</v>
@@ -783,241 +769,227 @@
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
       <c r="G7" s="9" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="11"/>
       <c r="J7" s="9" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
       <c r="M7" s="9" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="11"/>
       <c r="P7" s="9" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="11"/>
       <c r="S7" s="9" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="T7" s="10"/>
       <c r="U7" s="11"/>
       <c r="V7" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="W7" s="10"/>
       <c r="X7" s="11"/>
       <c r="Y7" s="9" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="Z7" s="10"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AC7" s="10"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="9" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AF7" s="10"/>
       <c r="AG7" s="11"/>
-      <c r="AH7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI7" s="10"/>
-      <c r="AJ7" s="11"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AD8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AF8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AG8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="X9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="Y9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="Z9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="AA9" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="V9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="X9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA9" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="AB9" s="7" t="s">
         <v>48</v>
@@ -1029,26 +1001,17 @@
         <v>50</v>
       </c>
       <c r="AE9" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AF9" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH9" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="AI9" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ9" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
@@ -1060,7 +1023,6 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="AB7:AD7"/>
     <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AH7:AJ7"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:L7"/>

</xml_diff>